<commit_message>
Added alt part id to BOM
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9881FB6A-3825-44DA-8C25-6DDF2A05FD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A22BD99-3049-48A7-AD96-C72811784B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
   <si>
     <t>A1</t>
   </si>
@@ -85,9 +96,6 @@
     <t>U8</t>
   </si>
   <si>
-    <t>74AHC1G08</t>
-  </si>
-  <si>
     <t>Part Number</t>
   </si>
   <si>
@@ -175,9 +183,6 @@
     <t>MIC29300-5.0WT</t>
   </si>
   <si>
-    <t>5v 3a Voltage Regulator - Linear</t>
-  </si>
-  <si>
     <t>"And" gate</t>
   </si>
   <si>
@@ -199,9 +204,6 @@
     <t>Developer recommends using 16-pin DIP socket</t>
   </si>
   <si>
-    <t>Developer recommends using 30-pin DIP socket</t>
-  </si>
-  <si>
     <t>Mount Size/Package</t>
   </si>
   <si>
@@ -365,12 +367,39 @@
   </si>
   <si>
     <t>MUX36S16IDWR</t>
+  </si>
+  <si>
+    <t>Developer recommends using 30-pin DIP</t>
+  </si>
+  <si>
+    <t>74AUC1G08</t>
+  </si>
+  <si>
+    <t>45F25RE</t>
+  </si>
+  <si>
+    <t>25Ω; ±1%; 5W</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>5v; 3a</t>
+  </si>
+  <si>
+    <t>Voltage Regulator - Linear</t>
+  </si>
+  <si>
+    <t>Substitute Part #</t>
+  </si>
+  <si>
+    <t>MIC29310-5.0WT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -921,6 +950,18 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -939,18 +980,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -965,18 +994,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:I28"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Label(s)" dataDxfId="4"/>
-    <tableColumn id="2" name="Type" dataDxfId="3"/>
-    <tableColumn id="3" name="Value(s)" dataDxfId="2"/>
-    <tableColumn id="4" name="Part Number"/>
-    <tableColumn id="5" name="Mounting Type"/>
-    <tableColumn id="6" name="Mount Size/Package" dataDxfId="1"/>
-    <tableColumn id="7" name="Quantity"/>
-    <tableColumn id="8" name="Price Est." dataCellStyle="Currency"/>
-    <tableColumn id="9" name="Notes"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:J29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value(s)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Part Number"/>
+    <tableColumn id="11" xr3:uid="{DB8C0E2A-802A-407B-B11F-AE676828C3DF}" name="Substitute Part #"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mounting Type"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Mount Size/Package" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Price Est." dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1278,11 +1308,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,71 +1320,74 @@
     <col min="1" max="1" width="68.28515625" customWidth="1"/>
     <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="46.42578125" customWidth="1"/>
+    <col min="4" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="8">
         <v>10.38</v>
       </c>
-      <c r="I2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1362,51 +1395,53 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3">
+        <v>95</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>0.22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4">
+        <v>63</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4">
         <v>9</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <v>1.17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1414,25 +1449,26 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5">
+        <v>98</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I5" s="8">
         <v>0.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1440,562 +1476,594 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6">
+        <v>99</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>0.71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7">
         <v>12</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>2.48</v>
       </c>
-      <c r="I7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8">
+        <v>87</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>0.78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9">
         <v>3</v>
       </c>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10">
+        <v>88</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10">
         <v>3</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <v>1.38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11">
         <v>6</v>
       </c>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13">
+        <v>108</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13">
         <v>8</v>
       </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="8">
         <v>0.35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15">
         <v>3</v>
       </c>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16">
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16">
         <v>1</v>
       </c>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18" s="8">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18">
-        <v>3</v>
-      </c>
-      <c r="H18" s="8">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" s="8">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19">
+      <c r="B20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20">
+        <v>17</v>
+      </c>
+      <c r="I20" s="8">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21">
         <v>3</v>
       </c>
-      <c r="H19" s="8">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="I21" s="8">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G20">
-        <v>17</v>
-      </c>
-      <c r="H20" s="8">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21" s="8">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22" s="8">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G23">
+        <v>81</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23">
         <v>1</v>
       </c>
-      <c r="H23" s="8">
-        <v>6.11</v>
-      </c>
-      <c r="I23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="8">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24">
+        <v>111</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24">
         <v>1</v>
       </c>
-      <c r="H24" s="8">
-        <v>9.31</v>
-      </c>
-      <c r="I24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="8">
+        <v>6.11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25" s="8">
-        <v>1.26</v>
-      </c>
-      <c r="I25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" s="8">
+        <v>9.31</v>
+      </c>
+      <c r="J25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26" s="8">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" s="8">
+        <v>1.26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" s="8">
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E27" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27">
+      <c r="C29" s="2"/>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29">
         <v>1</v>
       </c>
-      <c r="H27" s="8">
-        <v>4.26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28" s="8">
+      <c r="I29" s="8">
         <v>0.53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6">
-        <f>SUM(G2:G28)</f>
-        <v>88</v>
-      </c>
-      <c r="H29" s="9">
-        <f>SUM(H2:H28)</f>
-        <v>48.39</v>
-      </c>
-      <c r="I29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6">
+        <f>SUM(H2:H29)</f>
+        <v>89</v>
+      </c>
+      <c r="I30" s="9">
+        <f>SUM(I2:I29)</f>
+        <v>50.129999999999995</v>
+      </c>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -2057,20 +2125,20 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
@@ -2082,30 +2150,30 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
@@ -2176,6 +2244,11 @@
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made PCB adjustments to remove separate 5v power
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A22BD99-3049-48A7-AD96-C72811784B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856B4649-6080-4E61-9B0B-463D1E01CFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
   <si>
     <t>A1</t>
   </si>
@@ -48,9 +48,6 @@
     <t>C7</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>Rectifier Diode</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>J11</t>
   </si>
   <si>
-    <t>J26</t>
-  </si>
-  <si>
     <t>JP1</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>TC7SU04F</t>
   </si>
   <si>
-    <t>U7</t>
-  </si>
-  <si>
     <t>U8</t>
   </si>
   <si>
@@ -111,36 +102,15 @@
     <t>C2, C3, C4, C5, C6, C8, C9, C11, C13</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>J1, J5</t>
-  </si>
-  <si>
     <t>J2, J3, J4</t>
   </si>
   <si>
-    <t>J6, J9, J12</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
     <t>Price Est.</t>
   </si>
   <si>
-    <t>J7, J15, J16, J17, J18, J19</t>
-  </si>
-  <si>
-    <t>J10, J20, J21, J22, J23, J24, J25, J27</t>
-  </si>
-  <si>
-    <t>J13, J14, J28</t>
-  </si>
-  <si>
     <t>P1, P2, P3</t>
   </si>
   <si>
@@ -150,9 +120,6 @@
     <t>TIP120</t>
   </si>
   <si>
-    <t>R4, R5, R7, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R23, R24, R26, R27</t>
-  </si>
-  <si>
     <t>R8, R23, R28</t>
   </si>
   <si>
@@ -243,21 +210,9 @@
     <t>Generic shrouded header - 6 pins (2 rows)</t>
   </si>
   <si>
-    <t>male header thing 2 pin (1 row)</t>
-  </si>
-  <si>
-    <t>male header thing 3 pins (1 row)</t>
-  </si>
-  <si>
-    <t>male header thing 4 pins (1 row)</t>
-  </si>
-  <si>
     <t>Generic shrouded header - 8 pins (2 rows)</t>
   </si>
   <si>
-    <t>male header motor thing (1 row)</t>
-  </si>
-  <si>
     <t>Generic shrouded header - 16 pins (2 rows)</t>
   </si>
   <si>
@@ -369,9 +324,6 @@
     <t>MUX36S16IDWR</t>
   </si>
   <si>
-    <t>Developer recommends using 30-pin DIP</t>
-  </si>
-  <si>
     <t>74AUC1G08</t>
   </si>
   <si>
@@ -394,6 +346,66 @@
   </si>
   <si>
     <t>MIC29310-5.0WT</t>
+  </si>
+  <si>
+    <t>U7, U9</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13</t>
+  </si>
+  <si>
+    <t>R4, R5, R7, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31</t>
+  </si>
+  <si>
+    <t>C12, C14</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>male header 2 pin (1 row)</t>
+  </si>
+  <si>
+    <t>male header 4 pins (1 row)</t>
+  </si>
+  <si>
+    <t>male header 3 pins (1 row)</t>
+  </si>
+  <si>
+    <t>male header 5 pins (1 row)</t>
+  </si>
+  <si>
+    <t>J6, J7, J12</t>
+  </si>
+  <si>
+    <t>J10, J13, J14</t>
+  </si>
+  <si>
+    <t>J15, J16, J17, J18, J19, J20</t>
+  </si>
+  <si>
+    <t>J8, J9, J21, J22, J23, J24, J25, J26</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Comes in lot</t>
+  </si>
+  <si>
+    <t>Comes in a lot with other KF2510 connectors.</t>
+  </si>
+  <si>
+    <t>Comes in lot; other parts using DE37566 can use parts from this bulk order.</t>
+  </si>
+  <si>
+    <t>Developer recommends using 30-pin DIP socket. DE37566 pins (mentioned below) may need to be used.</t>
   </si>
 </sst>
 </file>
@@ -881,7 +893,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -892,16 +904,29 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="21"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="21" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="11" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -948,18 +973,39 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -994,19 +1040,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
   <autoFilter ref="A1:J29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value(s)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Part Number"/>
-    <tableColumn id="11" xr3:uid="{DB8C0E2A-802A-407B-B11F-AE676828C3DF}" name="Substitute Part #"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mounting Type"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Mount Size/Package" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Price Est." dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value(s)" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Part Number" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{DB8C0E2A-802A-407B-B11F-AE676828C3DF}" name="Substitute Part #" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mounting Type" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Mount Size/Package" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Price Est." dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1312,15 +1358,16 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="5" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
@@ -1330,725 +1377,795 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9">
+        <v>10.38</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.22</v>
+      </c>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="8">
+        <v>9</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1.17</v>
+      </c>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1.42</v>
+      </c>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="8">
+        <v>13</v>
+      </c>
+      <c r="I7" s="9">
+        <v>2.48</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8">
+        <v>3</v>
+      </c>
+      <c r="I9" s="9">
+        <v>6.99</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8">
+        <v>3</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1.38</v>
+      </c>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8">
+        <v>6</v>
+      </c>
+      <c r="I11" s="9">
+        <v>11.99</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8">
+        <v>8</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8">
+        <v>3</v>
+      </c>
+      <c r="I15" s="9">
+        <v>7.99</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8">
+        <v>3</v>
+      </c>
+      <c r="I18" s="9">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="8">
+        <v>3</v>
+      </c>
+      <c r="I19" s="9">
+        <v>2.25</v>
+      </c>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="8">
+        <v>18</v>
+      </c>
+      <c r="I20" s="9">
+        <v>2.54</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <v>1.74</v>
+      </c>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" s="8">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1.18</v>
+      </c>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9">
+        <v>6.11</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9">
+        <v>9.31</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="8">
+        <v>2</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1.26</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2">
+      <c r="G27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="8">
         <v>1</v>
       </c>
-      <c r="I2" s="8">
-        <v>10.38</v>
-      </c>
-      <c r="J2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="I27" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="8">
+        <v>2</v>
+      </c>
+      <c r="I28" s="9">
+        <v>8.52</v>
+      </c>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H29" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
-      </c>
-      <c r="I7" s="8">
-        <v>2.48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="8">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11">
-        <v>6</v>
-      </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13">
-        <v>8</v>
-      </c>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="I29" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18" s="8">
-        <v>2.5499999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="I19" s="8">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20">
-        <v>17</v>
-      </c>
-      <c r="I20" s="8">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21" s="8">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="8">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23" s="8">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" s="8">
-        <v>6.11</v>
-      </c>
-      <c r="J24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25" s="8">
-        <v>9.31</v>
-      </c>
-      <c r="J25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-      <c r="I26" s="8">
-        <v>1.26</v>
-      </c>
-      <c r="J26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27" s="8">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" t="s">
-        <v>120</v>
-      </c>
-      <c r="F28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28" s="8">
-        <v>4.26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29" s="8">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4">
         <f>SUM(H2:H29)</f>
-        <v>89</v>
-      </c>
-      <c r="I30" s="9">
+        <v>92</v>
+      </c>
+      <c r="I30" s="6">
         <f>SUM(I2:I29)</f>
-        <v>50.129999999999995</v>
-      </c>
-      <c r="J30" s="6"/>
+        <v>82.55</v>
+      </c>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
@@ -2057,12 +2174,12 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Replaced THT demux with 4 SMD demuxes to reduce cost
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856B4649-6080-4E61-9B0B-463D1E01CFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98537C15-84FF-41BF-AF43-574DBA9BB082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t>A1</t>
   </si>
@@ -72,9 +72,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>ULN2003A</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Label(s)</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C8, C9, C11, C13</t>
-  </si>
-  <si>
     <t>J2, J3, J4</t>
   </si>
   <si>
@@ -132,12 +126,6 @@
     <t>May have to use 28-pin SOIC to DIP adapter board</t>
   </si>
   <si>
-    <t>4-channel 1:2 demultiplexer</t>
-  </si>
-  <si>
-    <t>ADG333ABNZ</t>
-  </si>
-  <si>
     <t>Power/Stepper driver</t>
   </si>
   <si>
@@ -165,9 +153,6 @@
     <t>THT (read notes)</t>
   </si>
   <si>
-    <t>Developer recommends using 20-pin DIP socket</t>
-  </si>
-  <si>
     <t>Developer recommends using 16-pin DIP socket</t>
   </si>
   <si>
@@ -243,9 +228,6 @@
     <t>SMD (read notes)</t>
   </si>
   <si>
-    <t>DIP20</t>
-  </si>
-  <si>
     <t>DIP30</t>
   </si>
   <si>
@@ -406,6 +388,21 @@
   </si>
   <si>
     <t>Developer recommends using 30-pin DIP socket. DE37566 pins (mentioned below) may need to be used.</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>1:2 demultiplexer</t>
+  </si>
+  <si>
+    <t>SN74LVC1G18DBVR</t>
+  </si>
+  <si>
+    <t>U10, U11, U12, U13</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C6, C8, C9, C11, C13, C15, C16, C17, C18</t>
   </si>
 </sst>
 </file>
@@ -984,9 +981,6 @@
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1006,6 +1000,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1040,19 +1037,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value(s)" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Part Number" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{DB8C0E2A-802A-407B-B11F-AE676828C3DF}" name="Substitute Part #" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mounting Type" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Mount Size/Package" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Price Est." dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Value(s)" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Part Number" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{DB8C0E2A-802A-407B-B11F-AE676828C3DF}" name="Substitute Part #" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mounting Type" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Mount Size/Package" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Price Est." dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1358,7 +1355,7 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,34 +1374,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1412,18 +1409,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H2" s="8">
         <v>1</v>
@@ -1432,7 +1429,7 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1443,17 +1440,17 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1463,31 +1460,31 @@
       </c>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H4" s="8">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I4" s="9">
-        <v>1.17</v>
+        <v>1.23</v>
       </c>
       <c r="J4" s="8"/>
     </row>
@@ -1499,17 +1496,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
@@ -1521,23 +1518,23 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H6" s="8">
         <v>2</v>
@@ -1547,23 +1544,23 @@
       </c>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H7" s="8">
         <v>13</v>
@@ -1572,23 +1569,23 @@
         <v>2.48</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8">
@@ -1601,18 +1598,18 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8">
@@ -1622,23 +1619,23 @@
         <v>6.99</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
@@ -1651,18 +1648,18 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8">
@@ -1672,54 +1669,54 @@
         <v>11.99</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8">
         <v>8</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -1728,15 +1725,15 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8">
@@ -1749,18 +1746,18 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8">
@@ -1770,23 +1767,23 @@
         <v>7.99</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8">
@@ -1802,41 +1799,41 @@
         <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8">
         <v>1</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8">
@@ -1849,21 +1846,21 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H19" s="8">
         <v>3</v>
@@ -1873,25 +1870,25 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H20" s="8">
         <v>18</v>
@@ -1903,23 +1900,23 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H21" s="8">
         <v>3</v>
@@ -1931,20 +1928,20 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="8">
@@ -1964,14 +1961,14 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H23" s="8">
         <v>1</v>
@@ -1986,18 +1983,18 @@
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H24" s="8">
         <v>1</v>
@@ -2006,54 +2003,52 @@
         <v>6.11</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="H25" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I25" s="9">
-        <v>9.31</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>44</v>
-      </c>
+        <v>1.64</v>
+      </c>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H26" s="8">
         <v>2</v>
@@ -2062,26 +2057,26 @@
         <v>1.26</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H27" s="8">
         <v>1</v>
@@ -2093,25 +2088,25 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H28" s="8">
         <v>2</v>
@@ -2123,21 +2118,21 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H29" s="8">
         <v>1</v>
@@ -2149,7 +2144,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2159,11 +2154,11 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4">
         <f>SUM(H2:H29)</f>
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="I30" s="6">
         <f>SUM(I2:I29)</f>
-        <v>82.55</v>
+        <v>74.94</v>
       </c>
       <c r="J30" s="4"/>
     </row>
@@ -2174,12 +2169,12 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Address issues discovered after PCB revision testing
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98537C15-84FF-41BF-AF43-574DBA9BB082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA9AA84-A8B4-4FEF-ADB9-3C07089DD3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4035" yWindow="2190" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>TIP120</t>
   </si>
   <si>
-    <t>R8, R23, R28</t>
-  </si>
-  <si>
     <t>16:1 multiplexer</t>
   </si>
   <si>
@@ -336,12 +333,6 @@
     <t>J5</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13</t>
-  </si>
-  <si>
-    <t>R4, R5, R7, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31</t>
-  </si>
-  <si>
     <t>C12, C14</t>
   </si>
   <si>
@@ -402,14 +393,24 @@
     <t>U10, U11, U12, U13</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C8, C9, C11, C13, C15, C16, C17, C18</t>
+    <t>C2, C3, C4, C6, C8, C9, C11, C13, C15, C16, C17, C18</t>
+  </si>
+  <si>
+    <t>R5, R7, R8, R23, R28</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D13</t>
+  </si>
+  <si>
+    <t>R4, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31, R32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
@@ -890,7 +891,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -922,6 +923,9 @@
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1355,7 +1359,7 @@
   <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,22 +1381,22 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -1401,7 +1405,7 @@
         <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1417,10 +1421,10 @@
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" s="8">
         <v>1</v>
@@ -1429,7 +1433,7 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1440,17 +1444,17 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1462,29 +1466,29 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="9">
-        <v>1.23</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="J4" s="8"/>
     </row>
@@ -1496,17 +1500,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
@@ -1518,23 +1522,23 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="8">
         <v>2</v>
@@ -1546,46 +1550,46 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="8">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I7" s="9">
         <v>2.48</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8">
@@ -1601,15 +1605,15 @@
         <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8">
@@ -1619,23 +1623,23 @@
         <v>6.99</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
@@ -1648,18 +1652,18 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8">
@@ -1669,54 +1673,54 @@
         <v>11.99</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8">
         <v>8</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -1725,15 +1729,15 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8">
@@ -1746,18 +1750,18 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8">
@@ -1767,23 +1771,23 @@
         <v>7.99</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8">
@@ -1799,22 +1803,22 @@
         <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8">
         <v>1</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J17" s="8"/>
     </row>
@@ -1823,17 +1827,17 @@
         <v>24</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="D18" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8">
@@ -1857,10 +1861,10 @@
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H19" s="8">
         <v>3</v>
@@ -1872,76 +1876,76 @@
     </row>
     <row r="20" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="9">
-        <v>2.54</v>
+        <v>2.4</v>
       </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H21" s="8">
-        <v>3</v>
-      </c>
-      <c r="I21" s="9">
-        <v>0.33</v>
+        <v>5</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0.55000000000000004</v>
       </c>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="8">
@@ -1961,14 +1965,14 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H23" s="8">
         <v>1</v>
@@ -1983,18 +1987,18 @@
         <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H24" s="8">
         <v>1</v>
@@ -2003,26 +2007,26 @@
         <v>6.11</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H25" s="8">
         <v>4</v>
@@ -2034,10 +2038,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="8" t="s">
@@ -2045,10 +2049,10 @@
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="8">
         <v>2</v>
@@ -2057,7 +2061,7 @@
         <v>1.26</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2065,7 +2069,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="8" t="s">
@@ -2073,10 +2077,10 @@
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H27" s="8">
         <v>1</v>
@@ -2088,25 +2092,25 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" s="8">
         <v>2</v>
@@ -2121,18 +2125,18 @@
         <v>16</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H29" s="8">
         <v>1</v>
@@ -2144,7 +2148,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2154,11 +2158,11 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4">
         <f>SUM(H2:H29)</f>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I30" s="6">
         <f>SUM(I2:I29)</f>
-        <v>74.94</v>
+        <v>74.929999999999993</v>
       </c>
       <c r="J30" s="4"/>
     </row>
@@ -2169,12 +2173,12 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated board to V3
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA9AA84-A8B4-4FEF-ADB9-3C07089DD3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50946A64-C2C3-4242-8482-72E7F0DFEFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4035" yWindow="2190" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
   <si>
     <t>A1</t>
   </si>
@@ -63,12 +63,6 @@
     <t>Basic FET P-Channel</t>
   </si>
   <si>
-    <t>RL1</t>
-  </si>
-  <si>
-    <t>Relay</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
     <t>P1, P2, P3</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3</t>
-  </si>
-  <si>
     <t>TIP120</t>
   </si>
   <si>
@@ -210,12 +201,6 @@
     <t>DIP16</t>
   </si>
   <si>
-    <t>DPDT (2 Form C)</t>
-  </si>
-  <si>
-    <t>J104D2C5VDC.20S</t>
-  </si>
-  <si>
     <t>P160KN2-0QA25B10K</t>
   </si>
   <si>
@@ -306,15 +291,6 @@
     <t>74AUC1G08</t>
   </si>
   <si>
-    <t>45F25RE</t>
-  </si>
-  <si>
-    <t>25Ω; ±1%; 5W</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
     <t>5v; 3a</t>
   </si>
   <si>
@@ -399,10 +375,22 @@
     <t>R5, R7, R8, R23, R28</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D13</t>
-  </si>
-  <si>
-    <t>R4, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31, R32</t>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>1:2 demultiplexer (12v)</t>
+  </si>
+  <si>
+    <t>ISL43210IHZ-T7A</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>R4, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31, R32, R33</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1029,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1356,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,34 +1366,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1413,18 +1401,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H2" s="8">
         <v>1</v>
@@ -1433,7 +1421,7 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1444,17 +1432,17 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1466,23 +1454,23 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H4" s="8">
         <v>12</v>
@@ -1500,17 +1488,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
@@ -1522,23 +1510,23 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H6" s="8">
         <v>2</v>
@@ -1550,46 +1538,46 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H7" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="9">
         <v>2.48</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8">
@@ -1602,18 +1590,18 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8">
@@ -1623,23 +1611,23 @@
         <v>6.99</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
@@ -1652,18 +1640,18 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8">
@@ -1673,54 +1661,54 @@
         <v>11.99</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8">
         <v>8</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -1729,15 +1717,15 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8">
@@ -1750,18 +1738,18 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8">
@@ -1771,23 +1759,23 @@
         <v>7.99</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8">
@@ -1803,41 +1791,41 @@
         <v>8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8">
         <v>1</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8">
@@ -1850,77 +1838,77 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H19" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" s="9">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H20" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I20" s="9">
-        <v>2.4</v>
+        <v>2.54</v>
       </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H21" s="8">
         <v>5</v>
@@ -1932,27 +1920,27 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="11"/>
+        <v>34</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="H22" s="8">
         <v>1</v>
       </c>
       <c r="I22" s="9">
-        <v>1.74</v>
+        <v>2.92</v>
       </c>
       <c r="J22" s="8"/>
     </row>
@@ -1961,87 +1949,89 @@
         <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H23" s="8">
         <v>1</v>
       </c>
       <c r="I23" s="9">
-        <v>1.18</v>
-      </c>
-      <c r="J23" s="8"/>
+        <v>6.11</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="H24" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I24" s="9">
-        <v>6.11</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>29</v>
-      </c>
+        <v>1.64</v>
+      </c>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="H25" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I25" s="9">
-        <v>1.64</v>
-      </c>
-      <c r="J25" s="8"/>
+        <v>1.26</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="8" t="s">
@@ -2049,137 +2039,114 @@
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="H26" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="9">
-        <v>1.26</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>39</v>
-      </c>
+        <v>0.48</v>
+      </c>
+      <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>86</v>
+      </c>
       <c r="D27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="F27" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>74</v>
+        <v>33</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="H27" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" s="9">
-        <v>0.48</v>
+        <v>8.52</v>
       </c>
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4">
+        <f>SUM(H2:H28)</f>
         <v>95</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" s="8">
-        <v>2</v>
-      </c>
-      <c r="I28" s="9">
-        <v>8.52</v>
-      </c>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H29" s="8">
-        <v>1</v>
-      </c>
-      <c r="I29" s="9">
-        <v>0.53</v>
-      </c>
-      <c r="J29" s="8"/>
+      <c r="I29" s="6">
+        <f>SUM(I2:I28)</f>
+        <v>74.319999999999993</v>
+      </c>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4">
-        <f>SUM(H2:H29)</f>
-        <v>97</v>
-      </c>
-      <c r="I30" s="6">
-        <f>SUM(I2:I29)</f>
-        <v>74.929999999999993</v>
-      </c>
-      <c r="J30" s="4"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -2241,20 +2208,20 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
@@ -2266,30 +2233,30 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
@@ -2360,11 +2327,6 @@
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added alt part # for 6-pin plug
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50946A64-C2C3-4242-8482-72E7F0DFEFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3162A05-0AF5-495F-82FB-5E64C8A559C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="121">
   <si>
     <t>A1</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
+  </si>
+  <si>
+    <t>BHR-06-VUA</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1350,7 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1628,9 @@
       <c r="D10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="F10" s="8" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Removed parts from BOM
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3162A05-0AF5-495F-82FB-5E64C8A559C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EC6E09-A3F5-4E58-BDB7-96E682DAD788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
   <si>
     <t>A1</t>
   </si>
@@ -57,9 +57,6 @@
     <t>J11</t>
   </si>
   <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>Basic FET P-Channel</t>
   </si>
   <si>
@@ -372,9 +369,6 @@
     <t>C2, C3, C4, C6, C8, C9, C11, C13, C15, C16, C17, C18</t>
   </si>
   <si>
-    <t>R5, R7, R8, R23, R28</t>
-  </si>
-  <si>
     <t>Q1, Q2</t>
   </si>
   <si>
@@ -384,9 +378,6 @@
     <t>ISL43210IHZ-T7A</t>
   </si>
   <si>
-    <t>U14</t>
-  </si>
-  <si>
     <t>R4, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31, R32, R33</t>
   </si>
   <si>
@@ -394,6 +385,12 @@
   </si>
   <si>
     <t>BHR-06-VUA</t>
+  </si>
+  <si>
+    <t>R5, R7, R8, R23</t>
+  </si>
+  <si>
+    <t>U15</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1347,7 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,34 +1366,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,18 +1401,18 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="8">
         <v>1</v>
@@ -1424,7 +1421,7 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1435,17 +1432,17 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1457,23 +1454,23 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="8">
         <v>12</v>
@@ -1491,17 +1488,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
@@ -1513,23 +1510,23 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="8">
         <v>2</v>
@@ -1541,21 +1538,21 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="8">
         <v>10</v>
@@ -1564,23 +1561,23 @@
         <v>2.48</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8">
@@ -1593,18 +1590,18 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8">
@@ -1614,25 +1611,25 @@
         <v>6.99</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
@@ -1645,18 +1642,18 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8">
@@ -1666,54 +1663,54 @@
         <v>11.99</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8">
         <v>8</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -1722,15 +1719,15 @@
         <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8">
@@ -1743,18 +1740,18 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8">
@@ -1764,23 +1761,23 @@
         <v>7.99</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8">
@@ -1793,345 +1790,321 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="7"/>
       <c r="F17" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8">
-        <v>1</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>103</v>
+        <v>3</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2.5499999999999998</v>
       </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="8"/>
       <c r="H18" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="9">
-        <v>2.5499999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>54</v>
+      <c r="G19" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="H19" s="8">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="I19" s="9">
-        <v>1.5</v>
+        <v>2.54</v>
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" s="8">
-        <v>18</v>
-      </c>
-      <c r="I20" s="9">
-        <v>2.54</v>
+        <v>4</v>
+      </c>
+      <c r="I20" s="13">
+        <v>0.52</v>
       </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="H21" s="8">
-        <v>5</v>
-      </c>
-      <c r="I21" s="13">
-        <v>0.55000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>2.92</v>
       </c>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="H22" s="8">
         <v>1</v>
       </c>
       <c r="I22" s="9">
-        <v>2.92</v>
-      </c>
-      <c r="J22" s="8"/>
+        <v>6.11</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="H23" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I23" s="9">
-        <v>6.11</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>26</v>
-      </c>
+        <v>1.64</v>
+      </c>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
         <v>34</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="H24" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I24" s="9">
-        <v>1.64</v>
-      </c>
-      <c r="J24" s="8"/>
+        <v>1.26</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H25" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" s="9">
-        <v>1.26</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>36</v>
-      </c>
+        <v>0.48</v>
+      </c>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="F26" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>69</v>
+        <v>32</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="H26" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="9">
-        <v>0.48</v>
+        <v>8.52</v>
       </c>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>86</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>89</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>54</v>
+      <c r="G27" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="H27" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="9">
-        <v>8.52</v>
+        <v>0.53</v>
       </c>
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1</v>
-      </c>
-      <c r="I28" s="9">
-        <v>0.53</v>
-      </c>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4">
-        <f>SUM(H2:H28)</f>
-        <v>95</v>
-      </c>
-      <c r="I29" s="6">
-        <f>SUM(I2:I28)</f>
-        <v>74.319999999999993</v>
-      </c>
-      <c r="J29" s="4"/>
+      <c r="A28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4">
+        <f>SUM(H2:H27)</f>
+        <v>93</v>
+      </c>
+      <c r="I28" s="6">
+        <f>SUM(I2:I27)</f>
+        <v>74.290000000000006</v>
+      </c>
+      <c r="J28" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
@@ -2140,12 +2113,12 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2335,7 +2308,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Removed potentiometers from PCB
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EC6E09-A3F5-4E58-BDB7-96E682DAD788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C364E12F-FA86-4C98-90FC-CB055DF7B02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="116">
   <si>
     <t>A1</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Price Est.</t>
   </si>
   <si>
-    <t>P1, P2, P3</t>
-  </si>
-  <si>
     <t>TIP120</t>
   </si>
   <si>
@@ -186,21 +183,12 @@
     <t>Generic shrouded header - 16 pins (2 rows)</t>
   </si>
   <si>
-    <t>Potentiometer</t>
-  </si>
-  <si>
-    <t>10kΩ</t>
-  </si>
-  <si>
     <t>TO220</t>
   </si>
   <si>
     <t>DIP16</t>
   </si>
   <si>
-    <t>P160KN2-0QA25B10K</t>
-  </si>
-  <si>
     <t>SOIC</t>
   </si>
   <si>
@@ -378,9 +366,6 @@
     <t>ISL43210IHZ-T7A</t>
   </si>
   <si>
-    <t>R4, R9, R10, R11, R12, R13, R14, R15, R18, R19, R20, R24, R26, R27, R30, R31, R32, R33</t>
-  </si>
-  <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
   </si>
   <si>
@@ -391,14 +376,16 @@
   </si>
   <si>
     <t>U15</t>
+  </si>
+  <si>
+    <t>R4, R9, R10, R11, R12, R13, R14, R15, R24, R26, R27, R30, R31, R32, R33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
@@ -890,11 +877,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="21"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="21" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="11" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -913,7 +895,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="21" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="21" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="21" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1029,8 +1020,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1344,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,22 +1360,22 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>19</v>
@@ -1393,733 +1384,712 @@
         <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>10.38</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="5">
+        <v>12</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1.42</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="5">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2.48</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5">
+        <v>3</v>
+      </c>
+      <c r="I9" s="6">
+        <v>6.99</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1.38</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6">
+        <v>11.99</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>8</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
+        <v>3</v>
+      </c>
+      <c r="I15" s="6">
+        <v>7.99</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.73</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="5">
+        <v>2</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="5">
+        <v>15</v>
+      </c>
+      <c r="I18" s="6">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="5">
+        <v>4</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="6">
+        <v>2.92</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="6">
+        <v>6.11</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="5">
+        <v>4</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="5">
+        <v>2</v>
+      </c>
+      <c r="I23" s="6">
+        <v>1.26</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="8">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="5">
         <v>1</v>
       </c>
-      <c r="I2" s="9">
-        <v>10.38</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="I24" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2</v>
+      </c>
+      <c r="I25" s="6">
+        <v>8.52</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="8">
-        <v>12</v>
-      </c>
-      <c r="I4" s="9">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0.26</v>
-      </c>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="8">
-        <v>2</v>
-      </c>
-      <c r="I6" s="9">
-        <v>1.42</v>
-      </c>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="8">
-        <v>10</v>
-      </c>
-      <c r="I7" s="9">
-        <v>2.48</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10" t="s">
+      <c r="I26" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0.39</v>
-      </c>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8">
-        <v>3</v>
-      </c>
-      <c r="I9" s="9">
-        <v>6.99</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12">
+        <f>SUM(H2:H26)</f>
+        <v>87</v>
+      </c>
+      <c r="I27" s="13">
+        <f>SUM(I2:I26)</f>
+        <v>71.52</v>
+      </c>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8">
-        <v>3</v>
-      </c>
-      <c r="I10" s="9">
-        <v>1.38</v>
-      </c>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
-        <v>6</v>
-      </c>
-      <c r="I11" s="9">
-        <v>11.99</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8">
-        <v>1</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8">
-        <v>8</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9">
-        <v>0.35</v>
-      </c>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8">
-        <v>3</v>
-      </c>
-      <c r="I15" s="9">
-        <v>7.99</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="12">
-        <v>0.73</v>
-      </c>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8">
-        <v>3</v>
-      </c>
-      <c r="I17" s="9">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="8">
-        <v>2</v>
-      </c>
-      <c r="I18" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="8">
-        <v>18</v>
-      </c>
-      <c r="I19" s="9">
-        <v>2.54</v>
-      </c>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="8">
-        <v>4</v>
-      </c>
-      <c r="I20" s="13">
-        <v>0.52</v>
-      </c>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="8">
-        <v>1</v>
-      </c>
-      <c r="I21" s="9">
-        <v>2.92</v>
-      </c>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="8">
-        <v>1</v>
-      </c>
-      <c r="I22" s="9">
-        <v>6.11</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="8">
-        <v>4</v>
-      </c>
-      <c r="I23" s="9">
-        <v>1.64</v>
-      </c>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="8">
-        <v>2</v>
-      </c>
-      <c r="I24" s="9">
-        <v>1.26</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="8">
-        <v>1</v>
-      </c>
-      <c r="I25" s="9">
-        <v>0.48</v>
-      </c>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="8">
-        <v>2</v>
-      </c>
-      <c r="I26" s="9">
-        <v>8.52</v>
-      </c>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="8">
-        <v>1</v>
-      </c>
-      <c r="I27" s="9">
-        <v>0.53</v>
-      </c>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4">
-        <f>SUM(H2:H27)</f>
-        <v>93</v>
-      </c>
-      <c r="I28" s="6">
-        <f>SUM(I2:I27)</f>
-        <v>74.290000000000006</v>
-      </c>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -2181,20 +2151,20 @@
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
@@ -2206,30 +2176,30 @@
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
@@ -2300,11 +2270,6 @@
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed play sensors from PCB
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C364E12F-FA86-4C98-90FC-CB055DF7B02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4CF025-37E4-47C9-8096-E455C8538D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -321,9 +321,6 @@
     <t>J15, J16, J17, J18, J19, J20</t>
   </si>
   <si>
-    <t>J8, J9, J21, J22, J23, J24, J25, J26</t>
-  </si>
-  <si>
     <t>J27</t>
   </si>
   <si>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t>R4, R9, R10, R11, R12, R13, R14, R15, R24, R26, R27, R30, R31, R32, R33</t>
+  </si>
+  <si>
+    <t>J8, J9, J24, J25, J26</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1338,7 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1412,7 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -1602,7 +1602,7 @@
         <v>6.99</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1617,7 +1617,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>31</v>
@@ -1654,7 +1654,7 @@
         <v>11.99</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1677,13 +1677,13 @@
         <v>1</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>91</v>
@@ -1698,10 +1698,10 @@
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1752,12 +1752,12 @@
         <v>7.99</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>49</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>45</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>45</v>
@@ -1863,21 +1863,21 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" s="5">
         <v>1</v>
@@ -1917,21 +1917,21 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H22" s="5">
         <v>4</v>
@@ -2063,7 +2063,7 @@
       <c r="G27" s="11"/>
       <c r="H27" s="12">
         <f>SUM(H2:H26)</f>
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I27" s="13">
         <f>SUM(I2:I26)</f>

</xml_diff>

<commit_message>
Nearly finalize PCB and BOM v0.4
</commit_message>
<xml_diff>
--- a/electrical/BOM.xlsx
+++ b/electrical/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5303CE26-5CDA-4C4B-8BF8-A9E907F91775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF28E79-4F36-4708-9A60-5A04F2F6AAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,50 +31,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
   <si>
     <t>A1</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>Electrolytic Capacitor</t>
   </si>
   <si>
     <t>Ceramic Capacitor</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>Rectifier Diode</t>
   </si>
   <si>
     <t>Screw terminal - 2 pins</t>
   </si>
   <si>
-    <t>J11</t>
-  </si>
-  <si>
     <t>Basic FET P-Channel</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>ULN2003A</t>
   </si>
   <si>
     <t>U5</t>
   </si>
   <si>
-    <t>TC7SU04F</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
     <t>Part Number</t>
   </si>
   <si>
@@ -87,9 +69,6 @@
     <t>Label(s)</t>
   </si>
   <si>
-    <t>J2, J3, J4</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -99,21 +78,12 @@
     <t>TIP120</t>
   </si>
   <si>
-    <t>16:1 multiplexer</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>Power/Stepper driver</t>
   </si>
   <si>
-    <t>U3, U4</t>
-  </si>
-  <si>
-    <t>Inverter</t>
-  </si>
-  <si>
     <t>MIC29300-5.0WT</t>
   </si>
   <si>
@@ -141,15 +111,9 @@
     <t>Type</t>
   </si>
   <si>
-    <t>1.0-10.0µF; 50V</t>
-  </si>
-  <si>
     <t>Value(s)</t>
   </si>
   <si>
-    <t>100 mil</t>
-  </si>
-  <si>
     <t>300 mil</t>
   </si>
   <si>
@@ -168,9 +132,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>Generic male header - 3 pins (1 row)</t>
-  </si>
-  <si>
     <t>Generic shrouded header - 6 pins (2 rows)</t>
   </si>
   <si>
@@ -186,9 +147,6 @@
     <t>DIP16</t>
   </si>
   <si>
-    <t>SOIC</t>
-  </si>
-  <si>
     <t>DIP30</t>
   </si>
   <si>
@@ -210,15 +168,9 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Price estimates are as of 4 Feb. 2022</t>
-  </si>
-  <si>
     <t>YXQJST-XH 4S</t>
   </si>
   <si>
-    <t>106CKR063M</t>
-  </si>
-  <si>
     <t>SC-74A, SOT-753</t>
   </si>
   <si>
@@ -258,15 +210,9 @@
     <t>KF2510 3-pin</t>
   </si>
   <si>
-    <t>DE37566</t>
-  </si>
-  <si>
     <t>Comes in packs of 25</t>
   </si>
   <si>
-    <t>MUX36S16IDWR</t>
-  </si>
-  <si>
     <t>74AUC1G08</t>
   </si>
   <si>
@@ -282,33 +228,15 @@
     <t>MIC29310-5.0WT</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>male header 2 pin (1 row)</t>
   </si>
   <si>
     <t>male header 4 pins (1 row)</t>
   </si>
   <si>
-    <t>male header 3 pins (1 row)</t>
-  </si>
-  <si>
     <t>male header 5 pins (1 row)</t>
   </si>
   <si>
-    <t>J6, J7, J12</t>
-  </si>
-  <si>
-    <t>J10, J13, J14</t>
-  </si>
-  <si>
-    <t>J27</t>
-  </si>
-  <si>
     <t>--</t>
   </si>
   <si>
@@ -318,12 +246,6 @@
     <t>Comes in a lot with other KF2510 connectors.</t>
   </si>
   <si>
-    <t>Comes in lot; other parts using DE37566 can use parts from this bulk order.</t>
-  </si>
-  <si>
-    <t>Developer recommends using 30-pin DIP socket. DE37566 pins (mentioned below) may need to be used.</t>
-  </si>
-  <si>
     <t>SOT-23-6</t>
   </si>
   <si>
@@ -333,46 +255,136 @@
     <t>SN74LVC1G18DBVR</t>
   </si>
   <si>
-    <t>U10, U11, U12, U13</t>
-  </si>
-  <si>
-    <t>C2, C3, C4, C6, C8, C9, C11, C13, C15, C16, C17, C18</t>
-  </si>
-  <si>
-    <t>1:2 demultiplexer (12v)</t>
-  </si>
-  <si>
-    <t>ISL43210IHZ-T7A</t>
-  </si>
-  <si>
     <t>BHR-06-VUA</t>
   </si>
   <si>
-    <t>U15</t>
-  </si>
-  <si>
     <t>C14</t>
   </si>
   <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
-  </si>
-  <si>
-    <t>J15, J17, J18, J19, J20</t>
-  </si>
-  <si>
-    <t>R5, R7, R23</t>
-  </si>
-  <si>
-    <t>R4, R9, R10, R11, R12, R13, R14, R15, R24, R26, R27, R30, R32, R33</t>
-  </si>
-  <si>
-    <t>J8, J9, J24, J25, J26, J28</t>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>100µF; 16v</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>C4, C13</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C7, C8, C9, C10, C11, C12</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>Take from MX1508 PCB</t>
+  </si>
+  <si>
+    <t>J1, J21</t>
+  </si>
+  <si>
+    <t>J5, J6, J18, J24, J25, J26, J27</t>
+  </si>
+  <si>
+    <t>J3, J4, J7, J8</t>
+  </si>
+  <si>
+    <t>J9, J12, J13, J14, J15, J16, J17, J20, J22, J23</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>male header - 3 pins (1 row)</t>
+  </si>
+  <si>
+    <t>Developer recommends using 30-pin DIP socket. DE37566 pins may need to be used.</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>J10, J11</t>
+  </si>
+  <si>
+    <t>J19</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3, Q4</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>220Ω</t>
+  </si>
+  <si>
+    <t>R5, R7, R8, R9, R11, R12, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25</t>
+  </si>
+  <si>
+    <t>R6, R10, R13, R14, R15, R41</t>
+  </si>
+  <si>
+    <t>RL1, RL2, RL3</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>J104D2C5VDC.20S</t>
+  </si>
+  <si>
+    <t>DPDT (2 Form C)</t>
+  </si>
+  <si>
+    <t>U8, U9, U10, U11</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U1, U6</t>
+  </si>
+  <si>
+    <t>8:1 multiplexer</t>
+  </si>
+  <si>
+    <t>Motor driver</t>
+  </si>
+  <si>
+    <t>MX1508</t>
+  </si>
+  <si>
+    <t>CD4051BE</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U2, U3</t>
+  </si>
+  <si>
+    <t>Price estimates are as of 3 Sept. 2022</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1026,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J31" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1329,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,53 +1363,53 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -1406,313 +1418,313 @@
         <v>10.38</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.22</v>
-      </c>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H4" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I4" s="6">
-        <v>1.1399999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
       </c>
       <c r="I5" s="6">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H6" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="6">
-        <v>0.71</v>
+        <v>1.3</v>
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H7" s="5">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I7" s="6">
-        <v>2.48</v>
+        <v>1.58</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="5">
         <v>1</v>
       </c>
-      <c r="I8" s="6">
-        <v>0.39</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="H9" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" s="6">
-        <v>6.99</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>95</v>
-      </c>
+        <v>0.82</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>104</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="5">
-        <v>2</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.96</v>
+        <v>7</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="F11" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I11" s="6">
-        <v>11.99</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>94</v>
-      </c>
+        <v>1.92</v>
+      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5">
@@ -1725,44 +1737,42 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
-        <v>3</v>
-      </c>
-      <c r="I15" s="6">
-        <v>7.99</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I15" s="6"/>
       <c r="J15" s="5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5">
@@ -1775,308 +1785,385 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H17" s="5">
+        <v>4</v>
+      </c>
+      <c r="I17" s="6">
+        <v>3.32</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5">
         <v>1</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="5">
         <v>1</v>
       </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="5">
-        <v>14</v>
-      </c>
-      <c r="I18" s="6">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="5">
-        <v>3</v>
-      </c>
-      <c r="I19" s="6">
-        <v>0.33</v>
-      </c>
+      <c r="I19" s="6"/>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5" t="s">
-        <v>103</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="5">
         <v>1</v>
       </c>
-      <c r="I20" s="6">
-        <v>2.92</v>
-      </c>
+      <c r="I20" s="6"/>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="D21" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G21" s="4"/>
       <c r="H21" s="5">
         <v>1</v>
       </c>
-      <c r="I21" s="6">
-        <v>6.11</v>
-      </c>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="4"/>
       <c r="F22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>97</v>
+        <v>21</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="H22" s="5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I22" s="6">
-        <v>1.64</v>
+        <v>2.29</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="H23" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I23" s="6">
-        <v>1.26</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.66</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>62</v>
+        <v>20</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="H24" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I24" s="6">
-        <v>0.48</v>
+        <v>3.93</v>
       </c>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>79</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>82</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G25" s="4"/>
       <c r="H25" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" s="6">
-        <v>4.7</v>
+        <v>0.79</v>
       </c>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="5">
+        <v>4</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="5">
+        <v>2</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="5">
+        <v>1</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="5">
+      <c r="C29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="5">
+        <v>2</v>
+      </c>
+      <c r="I29" s="6">
+        <v>9.4</v>
+      </c>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="5">
         <v>1</v>
       </c>
-      <c r="I26" s="6">
-        <v>0.53</v>
-      </c>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12">
-        <f>SUM(H2:H26)</f>
-        <v>79</v>
-      </c>
-      <c r="I27" s="13">
-        <f>SUM(I2:I26)</f>
-        <v>65.63</v>
-      </c>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="I30" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="A31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="12">
+        <f>SUM(H2:H30)</f>
+        <v>103</v>
+      </c>
+      <c r="I31" s="13">
+        <f>SUM(I2:I30)</f>
+        <v>40.92</v>
+      </c>
+      <c r="J31" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -2084,19 +2171,14 @@
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -2143,6 +2225,11 @@
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
@@ -2153,20 +2240,20 @@
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -2178,20 +2265,20 @@
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
@@ -2203,11 +2290,6 @@
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-    </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
@@ -2262,6 +2344,26 @@
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>